<commit_message>
updated BOM and PnP file
</commit_message>
<xml_diff>
--- a/spear-dev-board/BOM.xlsx
+++ b/spear-dev-board/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Download\pcb_designs\spear-dev-board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B33E65D-30FC-4DD0-8843-C712EEF258F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C55C3F6-0726-4922-8AE4-6F290CC95030}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
   <si>
     <t>Comment</t>
   </si>
@@ -109,9 +109,6 @@
     <t>0805_C</t>
   </si>
   <si>
-    <t>10K</t>
-  </si>
-  <si>
     <t>R2,R4,R8</t>
   </si>
   <si>
@@ -124,12 +121,6 @@
     <t>U1</t>
   </si>
   <si>
-    <t>SOT23-5</t>
-  </si>
-  <si>
-    <t>4.7k</t>
-  </si>
-  <si>
     <t>R11, R12</t>
   </si>
   <si>
@@ -139,46 +130,28 @@
     <t>X1,X2</t>
   </si>
   <si>
-    <t>5032_2P</t>
-  </si>
-  <si>
-    <t>0805_LED</t>
-  </si>
-  <si>
     <t>LED1,LED2</t>
   </si>
   <si>
     <t>Green</t>
   </si>
   <si>
-    <t>1.5k</t>
-  </si>
-  <si>
     <t>R7</t>
   </si>
   <si>
     <t>R9</t>
   </si>
   <si>
-    <t>100k</t>
-  </si>
-  <si>
     <t>R1, R3</t>
   </si>
   <si>
     <t>J1</t>
   </si>
   <si>
-    <t>1k</t>
-  </si>
-  <si>
     <t>R10,R13</t>
   </si>
   <si>
     <t>U$2</t>
-  </si>
-  <si>
-    <t>LQFP48</t>
   </si>
   <si>
     <t>STM32F103CBT6</t>
@@ -203,13 +176,46 @@
     <t>TLV73333PDBVR</t>
   </si>
   <si>
-    <t>10uF-25V</t>
-  </si>
-  <si>
     <t>SKRPABE010</t>
   </si>
   <si>
     <t>U-F-M5SW-Y-3</t>
+  </si>
+  <si>
+    <t>LED_0805</t>
+  </si>
+  <si>
+    <t>4.7kOhm</t>
+  </si>
+  <si>
+    <t>10kOhm</t>
+  </si>
+  <si>
+    <t>100Ohm</t>
+  </si>
+  <si>
+    <t>100kOhm</t>
+  </si>
+  <si>
+    <t>1kOhm</t>
+  </si>
+  <si>
+    <t>22Ohm</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>SOT-23-5</t>
+  </si>
+  <si>
+    <t>LQFP-48_7X7X05P</t>
+  </si>
+  <si>
+    <t>SMD-5032_2P</t>
+  </si>
+  <si>
+    <t>1.5kOhm</t>
   </si>
 </sst>
 </file>
@@ -258,12 +264,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
@@ -275,8 +275,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -289,8 +295,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -324,6 +336,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFD1D1D1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -333,7 +354,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -367,14 +388,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -658,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -686,13 +713,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>4</v>
@@ -713,11 +740,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="27.6">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>13</v>
@@ -727,8 +754,8 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="5">
-        <v>22</v>
+      <c r="A5" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>9</v>
@@ -742,10 +769,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>15</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>10</v>
@@ -753,65 +780,66 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="8" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="8" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" ht="15" thickBot="1">
       <c r="A9" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>24</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="14"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="8" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12">
-        <v>100</v>
+      <c r="A12" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>10</v>
@@ -819,29 +847,30 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="8" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="13" t="s">
-        <v>47</v>
+      <c r="A14" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>33</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="8" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>10</v>
@@ -849,36 +878,36 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="12" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="9" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="8" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>37</v>
+        <v>30</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="8" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>37</v>
+        <v>31</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated BOM for SPEEDY
</commit_message>
<xml_diff>
--- a/spear-dev-board/BOM.xlsx
+++ b/spear-dev-board/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Download\pcb_designs\spear-dev-board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C55C3F6-0726-4922-8AE4-6F290CC95030}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F78ACA-1A5C-47ED-9531-7394207E8D02}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>Comment</t>
   </si>
@@ -78,28 +78,16 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">C16133  </t>
-  </si>
-  <si>
     <t>100nF</t>
   </si>
   <si>
     <t>0603_C</t>
   </si>
   <si>
-    <t>C14663</t>
-  </si>
-  <si>
-    <t>C13585</t>
-  </si>
-  <si>
     <t>R5, R6</t>
   </si>
   <si>
     <t>0603_R</t>
-  </si>
-  <si>
-    <t>C22809</t>
   </si>
   <si>
     <t xml:space="preserve">C3, C10, C11, C12, C13, C14, C15, C16, C17
@@ -145,15 +133,9 @@
     <t>R1, R3</t>
   </si>
   <si>
-    <t>J1</t>
-  </si>
-  <si>
     <t>R10,R13</t>
   </si>
   <si>
-    <t>U$2</t>
-  </si>
-  <si>
     <t>STM32F103CBT6</t>
   </si>
   <si>
@@ -161,9 +143,6 @@
   </si>
   <si>
     <t>IC2</t>
-  </si>
-  <si>
-    <t>STM32F303CBT6</t>
   </si>
   <si>
     <t xml:space="preserve">C1, C2
@@ -173,36 +152,9 @@
     <t>C115360</t>
   </si>
   <si>
-    <t>TLV73333PDBVR</t>
-  </si>
-  <si>
-    <t>SKRPABE010</t>
-  </si>
-  <si>
-    <t>U-F-M5SW-Y-3</t>
-  </si>
-  <si>
     <t>LED_0805</t>
   </si>
   <si>
-    <t>4.7kOhm</t>
-  </si>
-  <si>
-    <t>10kOhm</t>
-  </si>
-  <si>
-    <t>100Ohm</t>
-  </si>
-  <si>
-    <t>100kOhm</t>
-  </si>
-  <si>
-    <t>1kOhm</t>
-  </si>
-  <si>
-    <t>22Ohm</t>
-  </si>
-  <si>
     <t>10uF</t>
   </si>
   <si>
@@ -215,7 +167,25 @@
     <t>SMD-5032_2P</t>
   </si>
   <si>
-    <t>1.5kOhm</t>
+    <t>STM32F303CCT6</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>4.7k</t>
+  </si>
+  <si>
+    <t>1.5k</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>me6211-3.3V</t>
   </si>
 </sst>
 </file>
@@ -686,7 +656,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -713,201 +683,185 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="41.4">
       <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" ht="27.6">
       <c r="A4" s="3" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="5" t="s">
-        <v>44</v>
+      <c r="A5" s="5">
+        <v>22</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>11</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="8" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" thickBot="1">
       <c r="A9" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="D9" s="14"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="8" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="10" t="s">
-        <v>41</v>
+      <c r="A12" s="10">
+        <v>100</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>26</v>
-      </c>
+      <c r="A14" s="11"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>28</v>
-      </c>
+      <c r="A16" s="12"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="8"/>
       <c r="D16" s="9" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="8" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="13" t="s">
         <v>31</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>